<commit_message>
added flaot and span to WBS
</commit_message>
<xml_diff>
--- a/Project Documents/WBS.xlsx
+++ b/Project Documents/WBS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>1. Fall Detection</t>
   </si>
@@ -164,9 +164,6 @@
     <t>7.3 Trend Analysis Test Scripts (3 days;7.1, 2.3)</t>
   </si>
   <si>
-    <t>7.2 Sister Application Test Scripts (5 days; 7.1, 5.6)</t>
-  </si>
-  <si>
     <t>7.1 Fall Detection Test Scripts (7 days; 6.6)</t>
   </si>
   <si>
@@ -195,6 +192,114 @@
   </si>
   <si>
     <t>2.2 Create Short-Term Analysis (10 days; 2.1)</t>
+  </si>
+  <si>
+    <t>2.2 Create Short-Term Analysis (10 days)</t>
+  </si>
+  <si>
+    <t>5.5 Add Update Records Activity (2 days)</t>
+  </si>
+  <si>
+    <t>5.3 Add Edit Profile Activity (2 days)</t>
+  </si>
+  <si>
+    <t>6.7 Application Settings (3 days)</t>
+  </si>
+  <si>
+    <t>2.3 Create Long-Term Analysis (7 days)</t>
+  </si>
+  <si>
+    <t>6.6 Post-Incident Symptom Recording (2 days)</t>
+  </si>
+  <si>
+    <t>6.8 UI Update (5 days)</t>
+  </si>
+  <si>
+    <t>7.1 Fall Detection Test Scripts (7 days)</t>
+  </si>
+  <si>
+    <t>7.3 Trend Analysis Test Scripts (3 days)</t>
+  </si>
+  <si>
+    <t>7.2 Sister Application Test Scripts (5 days)</t>
+  </si>
+  <si>
+    <t>Earliest: 0</t>
+  </si>
+  <si>
+    <t>Latest: 0</t>
+  </si>
+  <si>
+    <t>Earliest: 0 - 10                                            Span: 10</t>
+  </si>
+  <si>
+    <t>Earliest: 10 - 20                                            Span: 10</t>
+  </si>
+  <si>
+    <t>Earliest: 20 - 27                                            Span: 7</t>
+  </si>
+  <si>
+    <t>Earliest: 27 - 30                                            Span: 3</t>
+  </si>
+  <si>
+    <t>Earliest: 25 - 30                                            Span: 5</t>
+  </si>
+  <si>
+    <t>Earliest: 18 - 25                                          Span: 7</t>
+  </si>
+  <si>
+    <t>Earliest: 13 - 18                                            Span: 5</t>
+  </si>
+  <si>
+    <t>Earliest: 10 - 13                                            Span: 3</t>
+  </si>
+  <si>
+    <t>Earliest: 0 - 3                                            Span: 9</t>
+  </si>
+  <si>
+    <t>Earliest: 3 - 5                                            Span: 8</t>
+  </si>
+  <si>
+    <t>Earliest: 5 - 7                                            Span: 8</t>
+  </si>
+  <si>
+    <t>Latest: 0 - 10                                            Float: 0</t>
+  </si>
+  <si>
+    <t>Latest: 6 - 9                                            Float: 6</t>
+  </si>
+  <si>
+    <t>Latest: 10 - 13                                            Float: 0</t>
+  </si>
+  <si>
+    <t>Latest: 10 - 20                                            Float: 0</t>
+  </si>
+  <si>
+    <t>Latest: 20 - 27                                            Float: 0</t>
+  </si>
+  <si>
+    <t>Latest: 27 - 30                                            Float: 0</t>
+  </si>
+  <si>
+    <t>Latest: 25 - 30                                            Float: 0</t>
+  </si>
+  <si>
+    <t>Latest: 18 - 25                                            Float: 0</t>
+  </si>
+  <si>
+    <t>Latest: 13 - 18                                            Float: 0</t>
+  </si>
+  <si>
+    <t>Latest: 11 - 13                                            Float: 6</t>
+  </si>
+  <si>
+    <t>Earliest: 10 - 12                                            Span: 3</t>
+  </si>
+  <si>
+    <t>Latest: 11 - 13                                            Float: 1</t>
+  </si>
+  <si>
+    <t>Latest: 9 - 11                                            Float: 6</t>
   </si>
 </sst>
 </file>
@@ -227,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +348,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -297,6 +408,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,11 +433,11 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>2705100</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
@@ -342,8 +454,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="21107400" y="5229225"/>
-          <a:ext cx="638175" cy="742950"/>
+          <a:off x="22498050" y="3343275"/>
+          <a:ext cx="619125" cy="723900"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -725,9 +837,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -742,8 +854,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24460200" y="6877050"/>
-          <a:ext cx="647700" cy="714375"/>
+          <a:off x="25850850" y="4991100"/>
+          <a:ext cx="609600" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -971,13 +1083,13 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>2381250</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>133352</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>2562225</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -992,8 +1104,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="37623750" y="5276852"/>
-          <a:ext cx="228600" cy="638173"/>
+          <a:off x="39014400" y="3381375"/>
+          <a:ext cx="180975" cy="628651"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1069,15 +1181,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>2800350</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>2647950</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1092,8 +1204,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="35213925" y="6115050"/>
-          <a:ext cx="361950" cy="600075"/>
+          <a:off x="36452175" y="4114800"/>
+          <a:ext cx="190500" cy="685800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1516,10 +1628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72933AF0-CDD0-4E49-83CA-D8B15E03A031}">
-  <dimension ref="A1:AA32"/>
+  <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,10 +1696,10 @@
       <c r="C2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -1600,7 +1712,7 @@
         <v>31</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -1610,10 +1722,10 @@
       <c r="C3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1627,7 +1739,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1636,7 +1748,7 @@
       <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -1665,7 +1777,7 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -1675,16 +1787,16 @@
         <v>27</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>44</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -1698,16 +1810,16 @@
         <v>28</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>39</v>
       </c>
       <c r="S6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U6" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1727,7 +1839,7 @@
         <v>43</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U7" s="3" t="s">
         <v>45</v>
@@ -1746,42 +1858,112 @@
         <v>40</v>
       </c>
     </row>
+    <row r="17" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>68</v>
+      </c>
+      <c r="S17" t="s">
+        <v>69</v>
+      </c>
+      <c r="U17" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="18" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S18" s="6" t="s">
         <v>56</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>79</v>
+      </c>
+      <c r="S19" t="s">
+        <v>82</v>
+      </c>
+      <c r="U19" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>76</v>
+      </c>
+      <c r="S21" t="s">
+        <v>77</v>
+      </c>
+      <c r="U21" t="s">
+        <v>78</v>
+      </c>
+      <c r="X21" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="22" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q22" s="6" t="s">
         <v>39</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="U22" s="6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="X22" s="6" t="s">
-        <v>47</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>80</v>
+      </c>
+      <c r="S23" t="s">
+        <v>91</v>
+      </c>
+      <c r="U23" t="s">
+        <v>88</v>
+      </c>
+      <c r="X23" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q25" t="s">
+        <v>68</v>
+      </c>
+      <c r="S25" t="s">
+        <v>89</v>
+      </c>
+      <c r="W25" t="s">
+        <v>74</v>
+      </c>
       <c r="AA25" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="15:27" x14ac:dyDescent="0.25">
@@ -1789,20 +1971,49 @@
         <v>41</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="W26" s="6" t="s">
-        <v>49</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>79</v>
+      </c>
+      <c r="S27" t="s">
+        <v>90</v>
+      </c>
+      <c r="W27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="S29" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S30" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="S31" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Y32" s="6" t="s">
-        <v>46</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y33" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added project file for network diagram to git
</commit_message>
<xml_diff>
--- a/Project Documents/WBS.xlsx
+++ b/Project Documents/WBS.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\GitHub\StruggleAssist\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD488530-F183-4E25-84E4-E16D803BDD63}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530" xr2:uid="{87CD842D-696A-434A-B4F7-D555111B0833}"/>
   </bookViews>
@@ -400,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -409,6 +410,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1630,7 +1632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72933AF0-CDD0-4E49-83CA-D8B15E03A031}">
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O12" workbookViewId="0">
       <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
@@ -1660,7 +1662,7 @@
     <col min="27" max="27" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1689,7 +1691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1715,7 +1717,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1738,7 +1740,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1799,7 +1801,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1822,7 +1824,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1845,7 +1847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K8" s="3" t="s">
         <v>34</v>
       </c>
@@ -1853,9 +1855,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K9" s="3" t="s">
         <v>40</v>
+      </c>
+      <c r="X9" s="8">
+        <v>57666959</v>
       </c>
     </row>
     <row r="17" spans="15:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completed work plan, slightly updated WBS
</commit_message>
<xml_diff>
--- a/Project Documents/WBS.xlsx
+++ b/Project Documents/WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\GitHub\StruggleAssist\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD488530-F183-4E25-84E4-E16D803BDD63}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F911B037-2D70-448C-9AF4-8638D6DE92CE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530" xr2:uid="{87CD842D-696A-434A-B4F7-D555111B0833}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
   <si>
     <t>1. Fall Detection</t>
   </si>
@@ -99,39 +99,12 @@
     <t>5.5 Add Update Records Activity</t>
   </si>
   <si>
-    <t>6.1 Add Notification Bar View</t>
-  </si>
-  <si>
-    <t>6.2 Add Lock Screen View</t>
-  </si>
-  <si>
-    <t>6.3 Add Event Confirmation</t>
-  </si>
-  <si>
-    <t>6.4 Add Event Cancellation</t>
-  </si>
-  <si>
-    <t>6.5 Add Event Timeout</t>
-  </si>
-  <si>
     <t>3.3 Create Settings Data Persistence</t>
   </si>
   <si>
-    <t>6.6 Post-Incident Symptom Recording</t>
-  </si>
-  <si>
-    <t>7.1 Fall Detection Test Scripts</t>
-  </si>
-  <si>
-    <t>7.2 Sister Application Test Scripts</t>
-  </si>
-  <si>
     <t>5.6 Emergency Contact Account</t>
   </si>
   <si>
-    <t>6.7 Application Settings</t>
-  </si>
-  <si>
     <t>2.2 Create Short-Term Analysis</t>
   </si>
   <si>
@@ -141,15 +114,9 @@
     <t>2.1 Create Trend Analysis Algorithm</t>
   </si>
   <si>
-    <t>7.3 Trend Analysis Test Scripts</t>
-  </si>
-  <si>
     <t>5.4 Add View Records Activity (3 days)</t>
   </si>
   <si>
-    <t>6.8 UI Update</t>
-  </si>
-  <si>
     <t>5.6 Emergency Contact Account (10 days)</t>
   </si>
   <si>
@@ -301,6 +268,45 @@
   </si>
   <si>
     <t>Latest: 9 - 11                                            Float: 6</t>
+  </si>
+  <si>
+    <t>6. Quality Assurance</t>
+  </si>
+  <si>
+    <t>6.1 Fall Detection Test Scripts</t>
+  </si>
+  <si>
+    <t>6.3 Trend Analysis Test Scripts</t>
+  </si>
+  <si>
+    <t>5. User Interaction</t>
+  </si>
+  <si>
+    <t>5.7 Add Notification Bar View</t>
+  </si>
+  <si>
+    <t>5.8 Add Lock Screen View</t>
+  </si>
+  <si>
+    <t>5.9 Add Event Confirmation</t>
+  </si>
+  <si>
+    <t>5.10 Add Event Cancellation</t>
+  </si>
+  <si>
+    <t>5.11 Add Event Timeout</t>
+  </si>
+  <si>
+    <t>5.12 Post-Incident Symptom Recording</t>
+  </si>
+  <si>
+    <t>5.13 Application Settings</t>
+  </si>
+  <si>
+    <t>5.14 UI Update</t>
+  </si>
+  <si>
+    <t>6.2 Emergency Contact Account Test Scripts</t>
   </si>
 </sst>
 </file>
@@ -1632,8 +1638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72933AF0-CDD0-4E49-83CA-D8B15E03A031}">
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O12" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,9 +1652,9 @@
     <col min="6" max="6" width="4.28515625" customWidth="1"/>
     <col min="7" max="7" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" customWidth="1"/>
-    <col min="11" max="11" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.28515625" customWidth="1"/>
     <col min="13" max="13" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30" customWidth="1"/>
@@ -1680,23 +1686,20 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
@@ -1707,14 +1710,11 @@
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>31</v>
+      <c r="K2" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>14</v>
@@ -1733,11 +1733,8 @@
       <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>32</v>
+      <c r="K3" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1745,10 +1742,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>18</v>
@@ -1756,11 +1753,8 @@
       <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>38</v>
+      <c r="K4" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>1</v>
@@ -1785,20 +1779,17 @@
       <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="O5" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1808,20 +1799,17 @@
       <c r="I6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="O6" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -1829,196 +1817,223 @@
         <v>12</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="K8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="K9" s="3" t="s">
-        <v>40</v>
+      <c r="I9" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="X9" s="8">
         <v>57666959</v>
       </c>
     </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I11" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I12" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I13" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I14" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I15" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="17" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q17" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="S17" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="U17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y17" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q18" s="6" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q19" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="S19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="U19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="Y19" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O21" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>65</v>
+      </c>
+      <c r="S21" t="s">
         <v>66</v>
       </c>
-      <c r="Q21" t="s">
-        <v>76</v>
-      </c>
-      <c r="S21" t="s">
-        <v>77</v>
-      </c>
       <c r="U21" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="X21" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="Q22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="S22" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="X22" s="6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O23" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="Q23" t="s">
+        <v>69</v>
+      </c>
+      <c r="S23" t="s">
         <v>80</v>
       </c>
-      <c r="S23" t="s">
-        <v>91</v>
-      </c>
       <c r="U23" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="X23" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q25" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="S25" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="W25" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="AA25" s="5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q26" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="W26" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q27" t="s">
+        <v>68</v>
+      </c>
+      <c r="S27" t="s">
         <v>79</v>
       </c>
-      <c r="S27" t="s">
-        <v>90</v>
-      </c>
       <c r="W27" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S29" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S30" s="6" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S31" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="Y31" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Y32" s="6" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="25:25" x14ac:dyDescent="0.25">
       <c r="Y33" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "completed work plan, slightly updated WBS"
This reverts commit 79dcecaee56dbb94115d404179e87990c4fe8915.
</commit_message>
<xml_diff>
--- a/Project Documents/WBS.xlsx
+++ b/Project Documents/WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\GitHub\StruggleAssist\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F911B037-2D70-448C-9AF4-8638D6DE92CE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD488530-F183-4E25-84E4-E16D803BDD63}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530" xr2:uid="{87CD842D-696A-434A-B4F7-D555111B0833}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>1. Fall Detection</t>
   </si>
@@ -99,12 +99,39 @@
     <t>5.5 Add Update Records Activity</t>
   </si>
   <si>
+    <t>6.1 Add Notification Bar View</t>
+  </si>
+  <si>
+    <t>6.2 Add Lock Screen View</t>
+  </si>
+  <si>
+    <t>6.3 Add Event Confirmation</t>
+  </si>
+  <si>
+    <t>6.4 Add Event Cancellation</t>
+  </si>
+  <si>
+    <t>6.5 Add Event Timeout</t>
+  </si>
+  <si>
     <t>3.3 Create Settings Data Persistence</t>
   </si>
   <si>
+    <t>6.6 Post-Incident Symptom Recording</t>
+  </si>
+  <si>
+    <t>7.1 Fall Detection Test Scripts</t>
+  </si>
+  <si>
+    <t>7.2 Sister Application Test Scripts</t>
+  </si>
+  <si>
     <t>5.6 Emergency Contact Account</t>
   </si>
   <si>
+    <t>6.7 Application Settings</t>
+  </si>
+  <si>
     <t>2.2 Create Short-Term Analysis</t>
   </si>
   <si>
@@ -114,9 +141,15 @@
     <t>2.1 Create Trend Analysis Algorithm</t>
   </si>
   <si>
+    <t>7.3 Trend Analysis Test Scripts</t>
+  </si>
+  <si>
     <t>5.4 Add View Records Activity (3 days)</t>
   </si>
   <si>
+    <t>6.8 UI Update</t>
+  </si>
+  <si>
     <t>5.6 Emergency Contact Account (10 days)</t>
   </si>
   <si>
@@ -268,45 +301,6 @@
   </si>
   <si>
     <t>Latest: 9 - 11                                            Float: 6</t>
-  </si>
-  <si>
-    <t>6. Quality Assurance</t>
-  </si>
-  <si>
-    <t>6.1 Fall Detection Test Scripts</t>
-  </si>
-  <si>
-    <t>6.3 Trend Analysis Test Scripts</t>
-  </si>
-  <si>
-    <t>5. User Interaction</t>
-  </si>
-  <si>
-    <t>5.7 Add Notification Bar View</t>
-  </si>
-  <si>
-    <t>5.8 Add Lock Screen View</t>
-  </si>
-  <si>
-    <t>5.9 Add Event Confirmation</t>
-  </si>
-  <si>
-    <t>5.10 Add Event Cancellation</t>
-  </si>
-  <si>
-    <t>5.11 Add Event Timeout</t>
-  </si>
-  <si>
-    <t>5.12 Post-Incident Symptom Recording</t>
-  </si>
-  <si>
-    <t>5.13 Application Settings</t>
-  </si>
-  <si>
-    <t>5.14 UI Update</t>
-  </si>
-  <si>
-    <t>6.2 Emergency Contact Account Test Scripts</t>
   </si>
 </sst>
 </file>
@@ -1638,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72933AF0-CDD0-4E49-83CA-D8B15E03A031}">
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="O12" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,9 +1646,9 @@
     <col min="6" max="6" width="4.28515625" customWidth="1"/>
     <col min="7" max="7" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" customWidth="1"/>
-    <col min="9" max="9" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" customWidth="1"/>
-    <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.28515625" customWidth="1"/>
     <col min="13" max="13" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30" customWidth="1"/>
@@ -1686,20 +1680,23 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
@@ -1710,11 +1707,14 @@
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>82</v>
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>14</v>
@@ -1733,8 +1733,11 @@
       <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>93</v>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1742,10 +1745,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>18</v>
@@ -1753,8 +1756,11 @@
       <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>83</v>
+      <c r="K4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>1</v>
@@ -1779,17 +1785,20 @@
       <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="K5" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="O5" s="3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1799,17 +1808,20 @@
       <c r="I6" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="K6" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="O6" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -1817,223 +1829,196 @@
         <v>12</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="U7" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K8" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I8" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="Q8" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I9" s="2" t="s">
-        <v>86</v>
+      <c r="K9" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="X9" s="8">
         <v>57666959</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I10" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I11" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I12" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I13" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I14" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I15" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
     <row r="17" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q17" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="S17" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="U17" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="Y17" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q18" s="6" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q19" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="S19" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="U19" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="Y19" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O21" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="Q21" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="S21" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="U21" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="X21" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Q22" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="S22" s="6" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="U22" s="6" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="X22" s="6" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O23" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="Q23" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="S23" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="U23" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="X23" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q25" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="S25" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="W25" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="AA25" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q26" s="6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="W26" s="6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q27" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="S27" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="W27" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S29" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S30" s="6" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S31" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="Y31" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Y32" s="6" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="25:25" x14ac:dyDescent="0.25">
       <c r="Y33" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished work plan and updated wbs
</commit_message>
<xml_diff>
--- a/Project Documents/WBS.xlsx
+++ b/Project Documents/WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\GitHub\StruggleAssist\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD488530-F183-4E25-84E4-E16D803BDD63}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F911B037-2D70-448C-9AF4-8638D6DE92CE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530" xr2:uid="{87CD842D-696A-434A-B4F7-D555111B0833}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
   <si>
     <t>1. Fall Detection</t>
   </si>
@@ -99,39 +99,12 @@
     <t>5.5 Add Update Records Activity</t>
   </si>
   <si>
-    <t>6.1 Add Notification Bar View</t>
-  </si>
-  <si>
-    <t>6.2 Add Lock Screen View</t>
-  </si>
-  <si>
-    <t>6.3 Add Event Confirmation</t>
-  </si>
-  <si>
-    <t>6.4 Add Event Cancellation</t>
-  </si>
-  <si>
-    <t>6.5 Add Event Timeout</t>
-  </si>
-  <si>
     <t>3.3 Create Settings Data Persistence</t>
   </si>
   <si>
-    <t>6.6 Post-Incident Symptom Recording</t>
-  </si>
-  <si>
-    <t>7.1 Fall Detection Test Scripts</t>
-  </si>
-  <si>
-    <t>7.2 Sister Application Test Scripts</t>
-  </si>
-  <si>
     <t>5.6 Emergency Contact Account</t>
   </si>
   <si>
-    <t>6.7 Application Settings</t>
-  </si>
-  <si>
     <t>2.2 Create Short-Term Analysis</t>
   </si>
   <si>
@@ -141,15 +114,9 @@
     <t>2.1 Create Trend Analysis Algorithm</t>
   </si>
   <si>
-    <t>7.3 Trend Analysis Test Scripts</t>
-  </si>
-  <si>
     <t>5.4 Add View Records Activity (3 days)</t>
   </si>
   <si>
-    <t>6.8 UI Update</t>
-  </si>
-  <si>
     <t>5.6 Emergency Contact Account (10 days)</t>
   </si>
   <si>
@@ -301,6 +268,45 @@
   </si>
   <si>
     <t>Latest: 9 - 11                                            Float: 6</t>
+  </si>
+  <si>
+    <t>6. Quality Assurance</t>
+  </si>
+  <si>
+    <t>6.1 Fall Detection Test Scripts</t>
+  </si>
+  <si>
+    <t>6.3 Trend Analysis Test Scripts</t>
+  </si>
+  <si>
+    <t>5. User Interaction</t>
+  </si>
+  <si>
+    <t>5.7 Add Notification Bar View</t>
+  </si>
+  <si>
+    <t>5.8 Add Lock Screen View</t>
+  </si>
+  <si>
+    <t>5.9 Add Event Confirmation</t>
+  </si>
+  <si>
+    <t>5.10 Add Event Cancellation</t>
+  </si>
+  <si>
+    <t>5.11 Add Event Timeout</t>
+  </si>
+  <si>
+    <t>5.12 Post-Incident Symptom Recording</t>
+  </si>
+  <si>
+    <t>5.13 Application Settings</t>
+  </si>
+  <si>
+    <t>5.14 UI Update</t>
+  </si>
+  <si>
+    <t>6.2 Emergency Contact Account Test Scripts</t>
   </si>
 </sst>
 </file>
@@ -1632,8 +1638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72933AF0-CDD0-4E49-83CA-D8B15E03A031}">
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O12" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,9 +1652,9 @@
     <col min="6" max="6" width="4.28515625" customWidth="1"/>
     <col min="7" max="7" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" customWidth="1"/>
-    <col min="11" max="11" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.28515625" customWidth="1"/>
     <col min="13" max="13" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30" customWidth="1"/>
@@ -1680,23 +1686,20 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
@@ -1707,14 +1710,11 @@
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>31</v>
+      <c r="K2" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>14</v>
@@ -1733,11 +1733,8 @@
       <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>32</v>
+      <c r="K3" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1745,10 +1742,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>18</v>
@@ -1756,11 +1753,8 @@
       <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>38</v>
+      <c r="K4" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>1</v>
@@ -1785,20 +1779,17 @@
       <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="O5" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1808,20 +1799,17 @@
       <c r="I6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="O6" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -1829,196 +1817,223 @@
         <v>12</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="K8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="K9" s="3" t="s">
-        <v>40</v>
+      <c r="I9" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="X9" s="8">
         <v>57666959</v>
       </c>
     </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I11" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I12" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I13" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I14" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I15" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="17" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q17" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="S17" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="U17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y17" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q18" s="6" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q19" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="S19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="U19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="Y19" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O21" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>65</v>
+      </c>
+      <c r="S21" t="s">
         <v>66</v>
       </c>
-      <c r="Q21" t="s">
-        <v>76</v>
-      </c>
-      <c r="S21" t="s">
-        <v>77</v>
-      </c>
       <c r="U21" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="X21" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="Q22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="S22" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="X22" s="6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O23" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="Q23" t="s">
+        <v>69</v>
+      </c>
+      <c r="S23" t="s">
         <v>80</v>
       </c>
-      <c r="S23" t="s">
-        <v>91</v>
-      </c>
       <c r="U23" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="X23" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q25" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="S25" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="W25" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="AA25" s="5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q26" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="W26" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q27" t="s">
+        <v>68</v>
+      </c>
+      <c r="S27" t="s">
         <v>79</v>
       </c>
-      <c r="S27" t="s">
-        <v>90</v>
-      </c>
       <c r="W27" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S29" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S30" s="6" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S31" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="Y31" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Y32" s="6" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="25:25" x14ac:dyDescent="0.25">
       <c r="Y33" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed work plan and wbs
</commit_message>
<xml_diff>
--- a/Project Documents/WBS.xlsx
+++ b/Project Documents/WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\GitHub\StruggleAssist\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F911B037-2D70-448C-9AF4-8638D6DE92CE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942F3605-8B98-4702-B7C8-4A383A9354A0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530" xr2:uid="{87CD842D-696A-434A-B4F7-D555111B0833}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
   <si>
     <t>1. Fall Detection</t>
   </si>
@@ -36,9 +36,6 @@
     <t>3. Data Persistence</t>
   </si>
   <si>
-    <t>4. Record Creation</t>
-  </si>
-  <si>
     <t>5. User Classes</t>
   </si>
   <si>
@@ -72,39 +69,9 @@
     <t>3.2 Create Event Records Database</t>
   </si>
   <si>
-    <t>4.1 Create Fall Detection Records</t>
-  </si>
-  <si>
-    <t>4.2 Create User Response Records</t>
-  </si>
-  <si>
-    <t>4.4 Create Location Recording Funcitonality</t>
-  </si>
-  <si>
-    <t>4.3 Create Video/Audio Recording Funcitonality</t>
-  </si>
-  <si>
-    <t>5.1 Add Create Profile Activity</t>
-  </si>
-  <si>
-    <t>5.2 Add Settings Activity</t>
-  </si>
-  <si>
-    <t>5.3 Add Edit Profile Activity</t>
-  </si>
-  <si>
-    <t>5.4 Add View Records Activity</t>
-  </si>
-  <si>
-    <t>5.5 Add Update Records Activity</t>
-  </si>
-  <si>
     <t>3.3 Create Settings Data Persistence</t>
   </si>
   <si>
-    <t>5.6 Emergency Contact Account</t>
-  </si>
-  <si>
     <t>2.2 Create Short-Term Analysis</t>
   </si>
   <si>
@@ -270,43 +237,61 @@
     <t>Latest: 9 - 11                                            Float: 6</t>
   </si>
   <si>
-    <t>6. Quality Assurance</t>
-  </si>
-  <si>
-    <t>6.1 Fall Detection Test Scripts</t>
-  </si>
-  <si>
-    <t>6.3 Trend Analysis Test Scripts</t>
-  </si>
-  <si>
-    <t>5. User Interaction</t>
-  </si>
-  <si>
-    <t>5.7 Add Notification Bar View</t>
-  </si>
-  <si>
-    <t>5.8 Add Lock Screen View</t>
-  </si>
-  <si>
-    <t>5.9 Add Event Confirmation</t>
-  </si>
-  <si>
-    <t>5.10 Add Event Cancellation</t>
-  </si>
-  <si>
-    <t>5.11 Add Event Timeout</t>
-  </si>
-  <si>
-    <t>5.12 Post-Incident Symptom Recording</t>
-  </si>
-  <si>
-    <t>5.13 Application Settings</t>
-  </si>
-  <si>
-    <t>5.14 UI Update</t>
-  </si>
-  <si>
-    <t>6.2 Emergency Contact Account Test Scripts</t>
+    <t>4. User Interaction</t>
+  </si>
+  <si>
+    <t>3.4 Create Fall Detection Records</t>
+  </si>
+  <si>
+    <t>3.5 Create User Response Records</t>
+  </si>
+  <si>
+    <t>3.6 Create Video/Audio Recording Funcitonality</t>
+  </si>
+  <si>
+    <t>3.7 Create Location Recording Funcitonality</t>
+  </si>
+  <si>
+    <t>4.1 Add Create Profile Activity</t>
+  </si>
+  <si>
+    <t>4.2 Add Settings Activity</t>
+  </si>
+  <si>
+    <t>4.3 Add Edit Profile Activity</t>
+  </si>
+  <si>
+    <t>4.4 Add View Records Activity</t>
+  </si>
+  <si>
+    <t>4.5 Add Update Records Activity</t>
+  </si>
+  <si>
+    <t>4.6 Emergency Contact Account</t>
+  </si>
+  <si>
+    <t>4.7 Add Notification Bar View</t>
+  </si>
+  <si>
+    <t>4.8 Add Lock Screen View</t>
+  </si>
+  <si>
+    <t>4.9 Add Event Confirmation</t>
+  </si>
+  <si>
+    <t>4.10 Add Event Cancellation</t>
+  </si>
+  <si>
+    <t>4.11 Add Event Timeout</t>
+  </si>
+  <si>
+    <t>4.12 Post-Incident Symptom Recording</t>
+  </si>
+  <si>
+    <t>4.13 Application Settings</t>
+  </si>
+  <si>
+    <t>4.14 UI Update</t>
   </si>
 </sst>
 </file>
@@ -1638,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72933AF0-CDD0-4E49-83CA-D8B15E03A031}">
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1633,7 @@
     <col min="2" max="2" width="4.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.28515625" customWidth="1"/>
     <col min="7" max="7" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" customWidth="1"/>
@@ -1682,358 +1667,347 @@
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="3"/>
       <c r="O2" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="3"/>
       <c r="O4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="S5" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="Q6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S6" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="U6" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I8" s="2" t="s">
-        <v>85</v>
+      <c r="E8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I9" s="2" t="s">
-        <v>86</v>
+      <c r="G9" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="X9" s="8">
         <v>57666959</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I10" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G11" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G12" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I11" s="2" t="s">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G15" s="3" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I12" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I13" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I14" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I15" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="17" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q17" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="S17" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="U17" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="Y17" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q18" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q19" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="S19" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="U19" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="Y19" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O21" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>54</v>
+      </c>
+      <c r="S21" t="s">
         <v>55</v>
       </c>
-      <c r="Q21" t="s">
-        <v>65</v>
-      </c>
-      <c r="S21" t="s">
-        <v>66</v>
-      </c>
       <c r="U21" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="X21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Q22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S22" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="X22" s="6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O23" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="Q23" t="s">
+        <v>58</v>
+      </c>
+      <c r="S23" t="s">
         <v>69</v>
       </c>
-      <c r="S23" t="s">
-        <v>80</v>
-      </c>
       <c r="U23" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="X23" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="15:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q25" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="S25" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="W25" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="AA25" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q26" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W26" s="6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q27" t="s">
+        <v>57</v>
+      </c>
+      <c r="S27" t="s">
         <v>68</v>
       </c>
-      <c r="S27" t="s">
-        <v>79</v>
-      </c>
       <c r="W27" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S29" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S30" s="6" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="15:27" x14ac:dyDescent="0.25">
       <c r="S31" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y31" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Y32" s="6" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="25:25" x14ac:dyDescent="0.25">
       <c r="Y33" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>